<commit_message>
First commit fall 24
</commit_message>
<xml_diff>
--- a/data-and-files/schedule_part1.xlsx
+++ b/data-and-files/schedule_part1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s12203\repos\ban400\data-and-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/work/repos/ban400/data-and-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2184EEE6-EB8F-4484-90E7-A3E5868F6B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219266F4-CC4B-F142-B43D-5E5C07BE8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="17520" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Lecture</t>
   </si>
@@ -71,67 +71,43 @@
     <t>[Assignment 2](assignment-02.qmd)</t>
   </si>
   <si>
-    <t>22.08 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>29.08 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>31.08 *08:15 - 10:00* (**LAB2**)</t>
-  </si>
-  <si>
-    <t>29.08 (*07:00*)</t>
-  </si>
-  <si>
-    <t>05.09 (*07:00*)</t>
-  </si>
-  <si>
-    <t>24.08 *08:15 - 10:00* (**LAB1**)</t>
-  </si>
-  <si>
-    <t>05.09 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
     <t>[Plotting](03-graphics.qmd)</t>
   </si>
   <si>
     <t>[Assignment 3](assignment-03.qmd)</t>
   </si>
   <si>
-    <t>07.09 *08:15 - 10:00* (**Aud J**)</t>
-  </si>
-  <si>
-    <t>12.09 (*07:00*)</t>
-  </si>
-  <si>
-    <t>12.09 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
     <t>[Functions and loops](04-functions-and-loops.qmd)</t>
   </si>
   <si>
     <t>[Assignment 4](assignment-04.qmd)</t>
   </si>
   <si>
-    <t>14.09 *08:15 - 10:00* (**Aud J**)</t>
-  </si>
-  <si>
-    <t>26.09 (*07:00*)</t>
-  </si>
-  <si>
     <t>19.09 *08:15 - 12:00* (**Aud M**)</t>
   </si>
   <si>
     <t>[Project organization](05-project-organization.qmd)</t>
   </si>
   <si>
-    <t>21.09 *08:15 - 10:00* (**Aud J**)</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
     <t>[Tidy data](02-data-wrangling.qmd)</t>
+  </si>
+  <si>
+    <t>27.08 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>03.09 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>10.09 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>17.09 *08:15 - 12:00* (**Aud M**)</t>
   </si>
 </sst>
 </file>
@@ -188,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -228,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -334,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -476,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -487,23 +463,23 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="32.125" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" customWidth="1"/>
     <col min="6" max="6" width="30.5" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -524,12 +500,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -541,21 +517,21 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -564,73 +540,73 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added seminar schedule H24
</commit_message>
<xml_diff>
--- a/data-and-files/schedule_part1.xlsx
+++ b/data-and-files/schedule_part1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/work/repos/ban400/data-and-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634FB10-2001-0D41-A2E3-C9EDF9E27DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388E06B-0E93-AC48-AB6D-A412C70F7CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
+    <workbookView xWindow="41100" yWindow="-2640" windowWidth="24860" windowHeight="17060" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Lecture</t>
   </si>
@@ -59,67 +59,79 @@
     <t>HO</t>
   </si>
   <si>
+    <t>[Introduction to R](01-intro-to-r.qmd)</t>
+  </si>
+  <si>
+    <t>OPMH</t>
+  </si>
+  <si>
+    <t>[Assignment 2](assignment-02.qmd)</t>
+  </si>
+  <si>
+    <t>[Plotting](03-graphics.qmd)</t>
+  </si>
+  <si>
+    <t>[Assignment 3](assignment-03.qmd)</t>
+  </si>
+  <si>
+    <t>[Functions and loops](04-functions-and-loops.qmd)</t>
+  </si>
+  <si>
+    <t>[Assignment 4](assignment-04.qmd)</t>
+  </si>
+  <si>
+    <t>[Project organization](05-project-organization.qmd)</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>[Tidy data](02-data-wrangling.qmd)</t>
+  </si>
+  <si>
+    <t>27.08 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>03.09 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>10.09 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>17.09 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>24.09 *08:15 - 12:00* (**Aud M**)</t>
+  </si>
+  <si>
+    <t>03.09.2024  (*07:00*)</t>
+  </si>
+  <si>
+    <t>10.09.2024 (*07:00*)</t>
+  </si>
+  <si>
+    <t>17.09.2024  (*07:00*)</t>
+  </si>
+  <si>
+    <t>24.09.2024  (*07:00*)</t>
+  </si>
+  <si>
     <t>[Assignment 1](assignment-01.qmd)</t>
   </si>
   <si>
-    <t>[Introduction to R](01-intro-to-r.qmd)</t>
-  </si>
-  <si>
-    <t>OPMH</t>
-  </si>
-  <si>
-    <t>[Assignment 2](assignment-02.qmd)</t>
-  </si>
-  <si>
-    <t>[Plotting](03-graphics.qmd)</t>
-  </si>
-  <si>
-    <t>[Assignment 3](assignment-03.qmd)</t>
-  </si>
-  <si>
-    <t>[Functions and loops](04-functions-and-loops.qmd)</t>
-  </si>
-  <si>
-    <t>[Assignment 4](assignment-04.qmd)</t>
-  </si>
-  <si>
-    <t>[Project organization](05-project-organization.qmd)</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>[Tidy data](02-data-wrangling.qmd)</t>
-  </si>
-  <si>
-    <t>27.08 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>03.09 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>10.09 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>17.09 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>24.09 *08:15 - 12:00* (**Aud M**)</t>
-  </si>
-  <si>
-    <t>03.09.2024  (*07:00*)</t>
-  </si>
-  <si>
-    <t>10.09.2024 (*07:00*)</t>
-  </si>
-  <si>
-    <t>17.09.2024  (*07:00*)</t>
-  </si>
-  <si>
-    <t>24.09.2024  (*07:00*)</t>
+    <t>29.08 *08:15 - 10:00* (**LAB2**)</t>
+  </si>
+  <si>
+    <t>05.09 *08:15 - 10:00* (**AUD G**)</t>
+  </si>
+  <si>
+    <t>12.09 *08:15 - 10:00* (**BORCH**)</t>
+  </si>
+  <si>
+    <t>19.09 *08:15 - 10:00* (**LAB2**)</t>
+  </si>
+  <si>
+    <t>26.09 *08:15 - 10:00* (**LAB2**)</t>
   </si>
 </sst>
 </file>
@@ -475,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A51BB1D-9DB0-9F4A-9922-FB93B5ED7B31}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -518,22 +530,22 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -541,22 +553,22 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -564,22 +576,22 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -587,22 +599,22 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -610,16 +622,16 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated lecture room 12.09
</commit_message>
<xml_diff>
--- a/data-and-files/schedule_part1.xlsx
+++ b/data-and-files/schedule_part1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/work/repos/ban400/data-and-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ban400\data-and-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388E06B-0E93-AC48-AB6D-A412C70F7CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A49E874-0C63-453F-A182-82F3DBCCCCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41100" yWindow="-2640" windowWidth="24860" windowHeight="17060" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -125,13 +125,13 @@
     <t>05.09 *08:15 - 10:00* (**AUD G**)</t>
   </si>
   <si>
-    <t>12.09 *08:15 - 10:00* (**BORCH**)</t>
-  </si>
-  <si>
     <t>19.09 *08:15 - 10:00* (**LAB2**)</t>
   </si>
   <si>
     <t>26.09 *08:15 - 10:00* (**LAB2**)</t>
+  </si>
+  <si>
+    <t>12.09 *08:15 - 10:00* (**AUD N**)</t>
   </si>
 </sst>
 </file>
@@ -189,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -229,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -335,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -488,10 +488,10 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -502,7 +502,7 @@
     <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -525,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>35</v>
       </c>
@@ -548,7 +548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>36</v>
       </c>
@@ -571,7 +571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>37</v>
       </c>
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>38</v>
       </c>
@@ -611,13 +611,13 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>39</v>
       </c>
@@ -631,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>